<commit_message>
Cambiadas las relaciones de las busquedas de pisos de los usuarios
</commit_message>
<xml_diff>
--- a/DataBase/Control de inserts.xlsx
+++ b/DataBase/Control de inserts.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="48">
   <si>
     <t>users</t>
   </si>
@@ -159,9 +159,6 @@
   </si>
   <si>
     <t>x</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
   </si>
   <si>
     <t>Tabla</t>
@@ -566,7 +563,7 @@
   <dimension ref="B3:D48"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -577,13 +574,13 @@
   <sheetData>
     <row r="3" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="D3" s="2" t="s">
         <v>47</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.25">
@@ -780,7 +777,7 @@
         <v>20</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D25" s="1"/>
     </row>

</xml_diff>